<commit_message>
Wont be using this PC anymore. pushing simply to keep whatever i did before.
</commit_message>
<xml_diff>
--- a/Experiments/Clustering algorithms.xlsx
+++ b/Experiments/Clustering algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik-Oslo\Documents\Crowding_GA_with_SLS\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE263576-CF81-49B7-8B49-7FCB5C65A4F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68042594-0D0C-4DDA-8F08-FD50B5EDC98D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="271">
   <si>
     <t>GA-innstillinger:</t>
   </si>
@@ -145,9 +145,6 @@
     <t>HDBSCAN</t>
   </si>
   <si>
-    <t>only variable = 2</t>
-  </si>
-  <si>
     <t>LSDBC</t>
   </si>
   <si>
@@ -827,6 +824,30 @@
   </si>
   <si>
     <t>3990.19(6311.09)</t>
+  </si>
+  <si>
+    <t>15127.52(20509.64)</t>
+  </si>
+  <si>
+    <t>minPts = 1</t>
+  </si>
+  <si>
+    <t>20.08(9.84)</t>
+  </si>
+  <si>
+    <t>404.98(254.03)</t>
+  </si>
+  <si>
+    <t>1906.78(728.11)</t>
+  </si>
+  <si>
+    <t>2732.87(630.9)</t>
+  </si>
+  <si>
+    <t>3695.74(4090.39)</t>
+  </si>
+  <si>
+    <t>802.39(779.75)</t>
   </si>
 </sst>
 </file>
@@ -1351,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FAFA54-A2D7-40DF-AA16-09B830FBBF6D}">
   <dimension ref="A2:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1383,7 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K2" s="1"/>
       <c r="O2" s="1" t="s">
@@ -1374,7 +1395,7 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O3" t="s">
         <v>33</v>
@@ -1385,7 +1406,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O4" t="s">
         <v>34</v>
@@ -1393,7 +1414,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1404,7 +1425,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1" t="s">
@@ -1414,7 +1435,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>27</v>
@@ -1423,7 +1444,7 @@
         <v>28</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>27</v>
@@ -1432,12 +1453,12 @@
         <v>28</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="U7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1448,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1457,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1472,10 +1493,10 @@
         <v>5</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1486,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1495,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1510,10 +1531,10 @@
         <v>10</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1524,7 +1545,7 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1533,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1548,10 +1569,10 @@
         <v>20</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1562,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1571,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -1586,10 +1607,10 @@
         <v>2</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1600,7 +1621,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -1609,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K12">
         <v>2</v>
@@ -1624,10 +1645,10 @@
         <v>5</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1638,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1647,7 +1668,7 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -1662,7 +1683,7 @@
         <v>8</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1673,7 +1694,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -1682,7 +1703,7 @@
         <v>2</v>
       </c>
       <c r="H14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K14">
         <v>3</v>
@@ -1697,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1708,7 +1729,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -1717,7 +1738,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K15">
         <v>3</v>
@@ -1732,7 +1753,7 @@
         <v>3</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1743,7 +1764,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -1752,7 +1773,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K16">
         <v>3</v>
@@ -1767,7 +1788,7 @@
         <v>4</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1778,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1787,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -1802,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -1813,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -1822,7 +1843,7 @@
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K18">
         <v>4</v>
@@ -1837,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1848,7 +1869,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -1857,7 +1878,7 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K19">
         <v>4</v>
@@ -1872,7 +1893,7 @@
         <v>20</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -1883,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F20">
         <v>5</v>
@@ -1892,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K20">
         <v>5</v>
@@ -1907,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -1918,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="2"/>
       <c r="F21" s="2">
@@ -1928,7 +1949,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K21" s="2">
         <v>5</v>
@@ -1943,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -1954,7 +1975,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="2"/>
       <c r="F22">
@@ -1964,7 +1985,7 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K22">
         <v>5</v>
@@ -1979,7 +2000,7 @@
         <v>4</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -1990,7 +2011,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D23" s="2"/>
       <c r="F23">
@@ -2000,7 +2021,7 @@
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K23">
         <v>6</v>
@@ -2015,7 +2036,7 @@
         <v>4</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -2026,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D24" s="2"/>
       <c r="F24">
@@ -2036,7 +2057,7 @@
         <v>6</v>
       </c>
       <c r="H24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K24">
         <v>6</v>
@@ -2051,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2062,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D25" s="2"/>
       <c r="F25">
@@ -2072,7 +2093,7 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K25">
         <v>6</v>
@@ -2087,7 +2108,7 @@
         <v>8</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -2098,7 +2119,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D26" s="2"/>
       <c r="F26">
@@ -2108,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="H26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K26">
         <v>7</v>
@@ -2123,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -2134,7 +2155,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D27" s="2"/>
       <c r="F27">
@@ -2144,7 +2165,7 @@
         <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K27">
         <v>7</v>
@@ -2159,7 +2180,7 @@
         <v>10</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -2170,7 +2191,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D28" s="2"/>
       <c r="F28">
@@ -2180,7 +2201,7 @@
         <v>16</v>
       </c>
       <c r="H28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K28">
         <v>7</v>
@@ -2195,7 +2216,7 @@
         <v>16</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2206,7 +2227,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="2"/>
       <c r="F29">
@@ -2216,7 +2237,7 @@
         <v>2</v>
       </c>
       <c r="H29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K29">
         <v>8</v>
@@ -2231,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2242,7 +2263,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D30" s="2"/>
       <c r="F30">
@@ -2252,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K30">
         <v>8</v>
@@ -2267,7 +2288,7 @@
         <v>3</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -2278,7 +2299,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D31" s="2"/>
       <c r="F31">
@@ -2288,7 +2309,7 @@
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K31">
         <v>8</v>
@@ -2303,7 +2324,7 @@
         <v>4</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -2314,7 +2335,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F32">
         <v>9</v>
@@ -2323,7 +2344,7 @@
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K32">
         <v>9</v>
@@ -2338,7 +2359,7 @@
         <v>10</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -2349,7 +2370,7 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F33">
         <v>9</v>
@@ -2358,7 +2379,7 @@
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K33">
         <v>9</v>
@@ -2373,7 +2394,7 @@
         <v>20</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -2384,7 +2405,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F34">
         <v>9</v>
@@ -2393,7 +2414,7 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K34">
         <v>9</v>
@@ -2408,7 +2429,7 @@
         <v>30</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2419,7 +2440,7 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F35">
         <v>10</v>
@@ -2428,7 +2449,7 @@
         <v>10</v>
       </c>
       <c r="H35" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K35">
         <v>10</v>
@@ -2443,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2454,7 +2475,7 @@
         <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F36">
         <v>10</v>
@@ -2463,7 +2484,7 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K36">
         <v>10</v>
@@ -2478,7 +2499,7 @@
         <v>20</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -2489,7 +2510,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F37">
         <v>10</v>
@@ -2498,7 +2519,7 @@
         <v>30</v>
       </c>
       <c r="H37" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K37">
         <v>10</v>
@@ -2513,7 +2534,7 @@
         <v>30</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2524,7 +2545,7 @@
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F38">
         <v>11</v>
@@ -2533,7 +2554,7 @@
         <v>10</v>
       </c>
       <c r="H38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K38">
         <v>11</v>
@@ -2548,7 +2569,7 @@
         <v>10</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2559,7 +2580,7 @@
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D39" s="2"/>
       <c r="F39">
@@ -2569,7 +2590,7 @@
         <v>20</v>
       </c>
       <c r="H39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K39">
         <v>11</v>
@@ -2584,7 +2605,7 @@
         <v>20</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2595,7 +2616,7 @@
         <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F40">
         <v>11</v>
@@ -2603,6 +2624,9 @@
       <c r="G40">
         <v>30</v>
       </c>
+      <c r="H40" t="s">
+        <v>265</v>
+      </c>
       <c r="K40">
         <v>11</v>
       </c>
@@ -2616,7 +2640,7 @@
         <v>30</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2627,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F41">
         <v>12</v>
@@ -2635,6 +2659,9 @@
       <c r="G41">
         <v>10</v>
       </c>
+      <c r="H41" t="s">
+        <v>266</v>
+      </c>
       <c r="K41">
         <v>12</v>
       </c>
@@ -2648,7 +2675,7 @@
         <v>10</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2659,7 +2686,7 @@
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F42">
         <v>12</v>
@@ -2667,6 +2694,9 @@
       <c r="G42">
         <v>20</v>
       </c>
+      <c r="H42" t="s">
+        <v>267</v>
+      </c>
       <c r="K42">
         <v>12</v>
       </c>
@@ -2680,7 +2710,7 @@
         <v>20</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2691,7 +2721,7 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F43">
         <v>12</v>
@@ -2699,6 +2729,9 @@
       <c r="G43">
         <v>30</v>
       </c>
+      <c r="H43" t="s">
+        <v>268</v>
+      </c>
       <c r="K43">
         <v>12</v>
       </c>
@@ -2712,7 +2745,7 @@
         <v>30</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2723,7 +2756,7 @@
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F44">
         <v>13</v>
@@ -2731,6 +2764,9 @@
       <c r="G44">
         <v>10</v>
       </c>
+      <c r="H44" t="s">
+        <v>270</v>
+      </c>
       <c r="K44">
         <v>13</v>
       </c>
@@ -2744,7 +2780,7 @@
         <v>10</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2755,7 +2791,7 @@
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F45">
         <v>13</v>
@@ -2763,6 +2799,9 @@
       <c r="G45">
         <v>20</v>
       </c>
+      <c r="H45" t="s">
+        <v>269</v>
+      </c>
       <c r="K45">
         <v>13</v>
       </c>
@@ -2776,7 +2815,7 @@
         <v>20</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2787,7 +2826,7 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F46">
         <v>13</v>
@@ -2796,7 +2835,7 @@
         <v>30</v>
       </c>
       <c r="H46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K46">
         <v>13</v>
@@ -2811,7 +2850,7 @@
         <v>30</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -2822,7 +2861,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F47">
         <v>14</v>
@@ -2831,7 +2870,7 @@
         <v>10</v>
       </c>
       <c r="H47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K47">
         <v>14</v>
@@ -2846,7 +2885,7 @@
         <v>10</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -2857,7 +2896,7 @@
         <v>20</v>
       </c>
       <c r="C48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F48">
         <v>14</v>
@@ -2866,7 +2905,7 @@
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K48">
         <v>14</v>
@@ -2881,7 +2920,7 @@
         <v>20</v>
       </c>
       <c r="Q48" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -2892,7 +2931,7 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F49">
         <v>14</v>
@@ -2901,7 +2940,7 @@
         <v>30</v>
       </c>
       <c r="H49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K49">
         <v>14</v>
@@ -2916,7 +2955,7 @@
         <v>30</v>
       </c>
       <c r="Q49" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2927,7 +2966,7 @@
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F50">
         <v>15</v>
@@ -2936,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="H50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K50">
         <v>15</v>
@@ -2951,7 +2990,7 @@
         <v>10</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -2962,7 +3001,7 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F51">
         <v>15</v>
@@ -2971,7 +3010,7 @@
         <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K51">
         <v>15</v>
@@ -2986,7 +3025,7 @@
         <v>20</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -2997,7 +3036,7 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F52">
         <v>15</v>
@@ -3005,6 +3044,9 @@
       <c r="G52">
         <v>30</v>
       </c>
+      <c r="H52" t="s">
+        <v>263</v>
+      </c>
       <c r="K52">
         <v>15</v>
       </c>
@@ -3018,7 +3060,7 @@
         <v>30</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -3026,15 +3068,15 @@
         <v>35</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>264</v>
       </c>
       <c r="O59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -3050,7 +3092,7 @@
         <v>28</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O62" s="1" t="s">
         <v>27</v>
@@ -3059,7 +3101,7 @@
         <v>28</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -3070,7 +3112,7 @@
         <v>5</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O63">
         <v>1</v>
@@ -3079,7 +3121,7 @@
         <v>5</v>
       </c>
       <c r="Q63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -3090,7 +3132,7 @@
         <v>10</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O64">
         <v>1</v>
@@ -3099,7 +3141,7 @@
         <v>10</v>
       </c>
       <c r="Q64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -3110,7 +3152,7 @@
         <v>20</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O65">
         <v>1</v>
@@ -3119,7 +3161,7 @@
         <v>20</v>
       </c>
       <c r="Q65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -3130,7 +3172,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O66">
         <v>2</v>
@@ -3139,7 +3181,7 @@
         <v>2</v>
       </c>
       <c r="Q66" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -3150,7 +3192,7 @@
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O67">
         <v>2</v>
@@ -3159,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="Q67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -3170,7 +3212,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O68">
         <v>2</v>
@@ -3179,7 +3221,7 @@
         <v>8</v>
       </c>
       <c r="Q68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -3190,7 +3232,7 @@
         <v>2</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O69">
         <v>3</v>
@@ -3199,7 +3241,7 @@
         <v>2</v>
       </c>
       <c r="Q69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -3210,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O70">
         <v>3</v>
@@ -3219,7 +3261,7 @@
         <v>3</v>
       </c>
       <c r="Q70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -3230,7 +3272,7 @@
         <v>4</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O71">
         <v>3</v>
@@ -3239,7 +3281,7 @@
         <v>4</v>
       </c>
       <c r="Q71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -3250,7 +3292,7 @@
         <v>5</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O72">
         <v>4</v>
@@ -3259,7 +3301,7 @@
         <v>5</v>
       </c>
       <c r="Q72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -3270,7 +3312,7 @@
         <v>10</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O73">
         <v>4</v>
@@ -3279,7 +3321,7 @@
         <v>10</v>
       </c>
       <c r="Q73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
@@ -3290,7 +3332,7 @@
         <v>20</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O74">
         <v>4</v>
@@ -3299,7 +3341,7 @@
         <v>20</v>
       </c>
       <c r="Q74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
@@ -3310,7 +3352,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O75">
         <v>5</v>
@@ -3319,7 +3361,7 @@
         <v>2</v>
       </c>
       <c r="Q75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -3330,7 +3372,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O76" s="2">
         <v>5</v>
@@ -3339,7 +3381,7 @@
         <v>3</v>
       </c>
       <c r="Q76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
@@ -3350,7 +3392,7 @@
         <v>4</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O77">
         <v>5</v>
@@ -3359,7 +3401,7 @@
         <v>4</v>
       </c>
       <c r="Q77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
@@ -3370,7 +3412,7 @@
         <v>4</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O78">
         <v>6</v>
@@ -3379,7 +3421,7 @@
         <v>4</v>
       </c>
       <c r="Q78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
@@ -3390,7 +3432,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O79">
         <v>6</v>
@@ -3399,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="Q79" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -3410,7 +3452,7 @@
         <v>8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O80">
         <v>6</v>
@@ -3419,7 +3461,7 @@
         <v>8</v>
       </c>
       <c r="Q80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
@@ -3430,7 +3472,7 @@
         <v>6</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O81">
         <v>7</v>
@@ -3439,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="Q81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
@@ -3450,7 +3492,7 @@
         <v>10</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O82">
         <v>7</v>
@@ -3459,7 +3501,7 @@
         <v>10</v>
       </c>
       <c r="Q82" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
@@ -3470,7 +3512,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O83">
         <v>7</v>
@@ -3479,7 +3521,7 @@
         <v>16</v>
       </c>
       <c r="Q83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
@@ -3490,7 +3532,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O84">
         <v>8</v>
@@ -3499,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="Q84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
@@ -3510,7 +3552,7 @@
         <v>3</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O85">
         <v>8</v>
@@ -3519,7 +3561,7 @@
         <v>3</v>
       </c>
       <c r="Q85" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
@@ -3530,7 +3572,7 @@
         <v>4</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O86">
         <v>8</v>
@@ -3539,7 +3581,7 @@
         <v>4</v>
       </c>
       <c r="Q86" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
@@ -3550,7 +3592,7 @@
         <v>10</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O87">
         <v>9</v>
@@ -3559,7 +3601,7 @@
         <v>10</v>
       </c>
       <c r="Q87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
@@ -3570,7 +3612,7 @@
         <v>20</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O88">
         <v>9</v>
@@ -3579,7 +3621,7 @@
         <v>20</v>
       </c>
       <c r="Q88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
@@ -3590,7 +3632,7 @@
         <v>30</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O89">
         <v>9</v>
@@ -3599,7 +3641,7 @@
         <v>30</v>
       </c>
       <c r="Q89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
@@ -3610,7 +3652,7 @@
         <v>10</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O90">
         <v>10</v>
@@ -3619,7 +3661,7 @@
         <v>10</v>
       </c>
       <c r="Q90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
@@ -3630,7 +3672,7 @@
         <v>20</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O91">
         <v>10</v>
@@ -3639,7 +3681,7 @@
         <v>20</v>
       </c>
       <c r="Q91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
@@ -3650,7 +3692,7 @@
         <v>30</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O92">
         <v>10</v>
@@ -3659,7 +3701,7 @@
         <v>30</v>
       </c>
       <c r="Q92" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
@@ -3670,7 +3712,7 @@
         <v>10</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O93">
         <v>11</v>
@@ -3679,7 +3721,7 @@
         <v>10</v>
       </c>
       <c r="Q93" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
@@ -3690,7 +3732,7 @@
         <v>20</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O94">
         <v>11</v>
@@ -3699,7 +3741,7 @@
         <v>20</v>
       </c>
       <c r="Q94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
@@ -3710,7 +3752,7 @@
         <v>30</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O95">
         <v>11</v>
@@ -3719,7 +3761,7 @@
         <v>30</v>
       </c>
       <c r="Q95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
@@ -3730,7 +3772,7 @@
         <v>10</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O96">
         <v>12</v>
@@ -3739,7 +3781,7 @@
         <v>10</v>
       </c>
       <c r="Q96" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -3750,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O97">
         <v>12</v>
@@ -3759,7 +3801,7 @@
         <v>20</v>
       </c>
       <c r="Q97" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -3770,7 +3812,7 @@
         <v>30</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O98">
         <v>12</v>
@@ -3779,7 +3821,7 @@
         <v>30</v>
       </c>
       <c r="Q98" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -3790,7 +3832,7 @@
         <v>10</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O99">
         <v>13</v>
@@ -3799,7 +3841,7 @@
         <v>10</v>
       </c>
       <c r="Q99" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -3810,7 +3852,7 @@
         <v>20</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O100">
         <v>13</v>
@@ -3819,7 +3861,7 @@
         <v>20</v>
       </c>
       <c r="Q100" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
@@ -3830,7 +3872,7 @@
         <v>30</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O101">
         <v>13</v>
@@ -3839,7 +3881,7 @@
         <v>30</v>
       </c>
       <c r="Q101" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
@@ -3850,7 +3892,7 @@
         <v>10</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O102">
         <v>14</v>
@@ -3859,7 +3901,7 @@
         <v>10</v>
       </c>
       <c r="Q102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
@@ -3870,7 +3912,7 @@
         <v>20</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O103">
         <v>14</v>
@@ -3879,7 +3921,7 @@
         <v>20</v>
       </c>
       <c r="Q103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
@@ -3890,7 +3932,7 @@
         <v>30</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O104">
         <v>14</v>
@@ -3899,7 +3941,7 @@
         <v>30</v>
       </c>
       <c r="Q104" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -3910,7 +3952,7 @@
         <v>10</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O105">
         <v>15</v>
@@ -3919,7 +3961,7 @@
         <v>10</v>
       </c>
       <c r="Q105" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
@@ -3930,7 +3972,7 @@
         <v>20</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O106">
         <v>15</v>
@@ -3939,7 +3981,7 @@
         <v>20</v>
       </c>
       <c r="Q106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
@@ -3950,7 +3992,7 @@
         <v>30</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O107">
         <v>15</v>
@@ -3959,7 +4001,7 @@
         <v>30</v>
       </c>
       <c r="Q107" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MEC is now the only clustering algorithm.
</commit_message>
<xml_diff>
--- a/Experiments/Clustering algorithms.xlsx
+++ b/Experiments/Clustering algorithms.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik-Oslo\Documents\Crowding_GA_with_SLS\Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredrik\Documents\Crowding_GA_with_SLS\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68042594-0D0C-4DDA-8F08-FD50B5EDC98D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894CD6F8-B10F-40F1-9264-0BF347A8648B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{859EC958-069D-41C2-971F-BA92C576E400}"/>
   </bookViews>
   <sheets>
     <sheet name="GA-innstillinger" sheetId="1" r:id="rId1"/>
     <sheet name="Eksperiment 1 - Klyngingsalgori" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1213,7 +1212,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FAFA54-A2D7-40DF-AA16-09B830FBBF6D}">
   <dimension ref="A2:U107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>